<commit_message>
Comparing Supplement Table 1
Things look good, but need to clean up and make prettier.
</commit_message>
<xml_diff>
--- a/datasets/intermediate/Ghandour-2024-Supplementary-Data.xlsx
+++ b/datasets/intermediate/Ghandour-2024-Supplementary-Data.xlsx
@@ -5,17 +5,33 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcu\Dropbox\UNMC\hrtl-invalid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\HRTL-2016-2022\datasets\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8692E8D0-7600-4C2D-9999-4EFDED13BEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB4A398-53FC-4C8E-A0D5-F6146474A62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23430" yWindow="1470" windowWidth="22950" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23085" yWindow="1125" windowWidth="22950" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$388</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -651,15 +667,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C384" sqref="C384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -686,7 +704,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -709,7 +727,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -732,7 +750,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -755,7 +773,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -778,7 +796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -801,7 +819,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -824,7 +842,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -847,7 +865,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -870,7 +888,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -893,7 +911,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -916,7 +934,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -939,7 +957,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -962,7 +980,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -985,7 +1003,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1026,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>53.9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1077,7 +1095,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1100,7 +1118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1123,7 +1141,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1169,7 +1187,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +1233,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1238,7 +1256,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1261,7 +1279,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1302,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1325,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1330,7 +1348,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1371,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1376,7 +1394,7 @@
         <v>52.4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1399,7 +1417,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1422,7 +1440,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1445,7 +1463,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1486,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1491,7 +1509,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1514,7 +1532,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1560,7 +1578,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1606,7 +1624,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1647,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1693,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1721,7 +1739,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -1767,7 +1785,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -1813,7 +1831,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -1836,7 +1854,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
@@ -1859,7 +1877,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +1900,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -1905,7 +1923,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1951,7 +1969,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -1997,7 +2015,7 @@
         <v>61.1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2038,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>28</v>
       </c>
@@ -2043,7 +2061,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>28</v>
       </c>
@@ -2066,7 +2084,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -2112,7 +2130,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -2135,7 +2153,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -2158,7 +2176,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -2204,7 +2222,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -2227,7 +2245,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -2250,7 +2268,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -2273,7 +2291,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -2296,7 +2314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -2319,7 +2337,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -2342,7 +2360,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2406,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -2411,7 +2429,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -2434,7 +2452,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -2457,7 +2475,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -2480,7 +2498,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -2503,7 +2521,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -2526,7 +2544,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -2549,7 +2567,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -2572,7 +2590,7 @@
         <v>56.7</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>30</v>
       </c>
@@ -2595,7 +2613,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>30</v>
       </c>
@@ -2618,7 +2636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>30</v>
       </c>
@@ -2641,7 +2659,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>30</v>
       </c>
@@ -2664,7 +2682,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>30</v>
       </c>
@@ -2687,7 +2705,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -2710,7 +2728,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2733,7 +2751,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2756,7 +2774,7 @@
         <v>42.2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2779,7 +2797,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -2802,7 +2820,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -2825,7 +2843,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>90</v>
       </c>
@@ -2848,7 +2866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>90</v>
       </c>
@@ -2871,7 +2889,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -2894,7 +2912,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>90</v>
       </c>
@@ -2917,7 +2935,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -2940,7 +2958,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>90</v>
       </c>
@@ -2963,7 +2981,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>90</v>
       </c>
@@ -2986,7 +3004,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -3009,7 +3027,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -3032,7 +3050,7 @@
         <v>55.8</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -3055,7 +3073,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -3078,7 +3096,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -3101,7 +3119,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>36</v>
       </c>
@@ -3124,7 +3142,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>36</v>
       </c>
@@ -3147,7 +3165,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>36</v>
       </c>
@@ -3170,7 +3188,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>36</v>
       </c>
@@ -3193,7 +3211,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3234,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>36</v>
       </c>
@@ -3239,7 +3257,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>36</v>
       </c>
@@ -3262,7 +3280,7 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>36</v>
       </c>
@@ -3285,7 +3303,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -3308,7 +3326,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>36</v>
       </c>
@@ -3331,7 +3349,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>36</v>
       </c>
@@ -3354,7 +3372,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>36</v>
       </c>
@@ -3377,7 +3395,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>38</v>
       </c>
@@ -3400,7 +3418,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>38</v>
       </c>
@@ -3423,7 +3441,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>38</v>
       </c>
@@ -3446,7 +3464,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>38</v>
       </c>
@@ -3469,7 +3487,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>38</v>
       </c>
@@ -3492,7 +3510,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>38</v>
       </c>
@@ -3515,7 +3533,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>38</v>
       </c>
@@ -3538,7 +3556,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>38</v>
       </c>
@@ -3561,7 +3579,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>38</v>
       </c>
@@ -3584,7 +3602,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>38</v>
       </c>
@@ -3607,7 +3625,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>38</v>
       </c>
@@ -3630,7 +3648,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>38</v>
       </c>
@@ -3653,7 +3671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>38</v>
       </c>
@@ -3676,7 +3694,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>38</v>
       </c>
@@ -3699,7 +3717,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>38</v>
       </c>
@@ -3722,7 +3740,7 @@
         <v>39.1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>40</v>
       </c>
@@ -3745,7 +3763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>40</v>
       </c>
@@ -3768,7 +3786,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>40</v>
       </c>
@@ -3791,7 +3809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>40</v>
       </c>
@@ -3814,7 +3832,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>40</v>
       </c>
@@ -3837,7 +3855,7 @@
         <v>45.1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>40</v>
       </c>
@@ -3860,7 +3878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>40</v>
       </c>
@@ -3883,7 +3901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>40</v>
       </c>
@@ -3906,7 +3924,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>40</v>
       </c>
@@ -3929,7 +3947,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>40</v>
       </c>
@@ -3952,7 +3970,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>40</v>
       </c>
@@ -3975,7 +3993,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>40</v>
       </c>
@@ -3998,7 +4016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>40</v>
       </c>
@@ -4021,7 +4039,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>40</v>
       </c>
@@ -4044,7 +4062,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>40</v>
       </c>
@@ -4067,7 +4085,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>42</v>
       </c>
@@ -4090,7 +4108,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -4113,7 +4131,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -4136,7 +4154,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>42</v>
       </c>
@@ -4159,7 +4177,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -4182,7 +4200,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>42</v>
       </c>
@@ -4205,7 +4223,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>42</v>
       </c>
@@ -4228,7 +4246,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>42</v>
       </c>
@@ -4251,7 +4269,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -4274,7 +4292,7 @@
         <v>42.6</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -4297,7 +4315,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -4320,7 +4338,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -4343,7 +4361,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>42</v>
       </c>
@@ -4366,7 +4384,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>42</v>
       </c>
@@ -4389,7 +4407,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -4412,7 +4430,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>44</v>
       </c>
@@ -4435,7 +4453,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>44</v>
       </c>
@@ -4458,7 +4476,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>44</v>
       </c>
@@ -4481,7 +4499,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>44</v>
       </c>
@@ -4504,7 +4522,7 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>44</v>
       </c>
@@ -4527,7 +4545,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>44</v>
       </c>
@@ -4550,7 +4568,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>44</v>
       </c>
@@ -4573,7 +4591,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>44</v>
       </c>
@@ -4596,7 +4614,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>44</v>
       </c>
@@ -4619,7 +4637,7 @@
         <v>48.2</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>44</v>
       </c>
@@ -4642,7 +4660,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>44</v>
       </c>
@@ -4665,7 +4683,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>44</v>
       </c>
@@ -4688,7 +4706,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>44</v>
       </c>
@@ -4711,7 +4729,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>44</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>44</v>
       </c>
@@ -4757,7 +4775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>46</v>
       </c>
@@ -4780,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>46</v>
       </c>
@@ -4803,7 +4821,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>46</v>
       </c>
@@ -4826,7 +4844,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>46</v>
       </c>
@@ -4849,7 +4867,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>46</v>
       </c>
@@ -4872,7 +4890,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>46</v>
       </c>
@@ -4895,7 +4913,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>46</v>
       </c>
@@ -4918,7 +4936,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>46</v>
       </c>
@@ -4941,7 +4959,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>46</v>
       </c>
@@ -4964,7 +4982,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>46</v>
       </c>
@@ -4987,7 +5005,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>46</v>
       </c>
@@ -5010,7 +5028,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>46</v>
       </c>
@@ -5033,7 +5051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>46</v>
       </c>
@@ -5056,7 +5074,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>46</v>
       </c>
@@ -5079,7 +5097,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>46</v>
       </c>
@@ -5102,7 +5120,7 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>48</v>
       </c>
@@ -5125,7 +5143,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>48</v>
       </c>
@@ -5148,7 +5166,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>48</v>
       </c>
@@ -5171,7 +5189,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>48</v>
       </c>
@@ -5194,7 +5212,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>48</v>
       </c>
@@ -5217,7 +5235,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>48</v>
       </c>
@@ -5240,7 +5258,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>48</v>
       </c>
@@ -5263,7 +5281,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>48</v>
       </c>
@@ -5286,7 +5304,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>48</v>
       </c>
@@ -5309,7 +5327,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>48</v>
       </c>
@@ -5332,7 +5350,7 @@
         <v>42.2</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>48</v>
       </c>
@@ -5355,7 +5373,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>48</v>
       </c>
@@ -5378,7 +5396,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>48</v>
       </c>
@@ -5401,7 +5419,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>48</v>
       </c>
@@ -5424,7 +5442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>48</v>
       </c>
@@ -5447,7 +5465,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>50</v>
       </c>
@@ -5470,7 +5488,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>50</v>
       </c>
@@ -5493,7 +5511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>50</v>
       </c>
@@ -5516,7 +5534,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>50</v>
       </c>
@@ -5539,7 +5557,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>50</v>
       </c>
@@ -5562,7 +5580,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>50</v>
       </c>
@@ -5585,7 +5603,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>50</v>
       </c>
@@ -5608,7 +5626,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>50</v>
       </c>
@@ -5631,7 +5649,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>50</v>
       </c>
@@ -5654,7 +5672,7 @@
         <v>41.4</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>50</v>
       </c>
@@ -5677,7 +5695,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>50</v>
       </c>
@@ -5700,7 +5718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>50</v>
       </c>
@@ -5723,7 +5741,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>50</v>
       </c>
@@ -5746,7 +5764,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>50</v>
       </c>
@@ -5769,7 +5787,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>50</v>
       </c>
@@ -5792,7 +5810,7 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>52</v>
       </c>
@@ -5815,7 +5833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>52</v>
       </c>
@@ -5838,7 +5856,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>52</v>
       </c>
@@ -5861,7 +5879,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>52</v>
       </c>
@@ -5884,7 +5902,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>52</v>
       </c>
@@ -5907,7 +5925,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>52</v>
       </c>
@@ -5930,7 +5948,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>52</v>
       </c>
@@ -5953,7 +5971,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>52</v>
       </c>
@@ -5976,7 +5994,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>52</v>
       </c>
@@ -5999,7 +6017,7 @@
         <v>48.7</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>52</v>
       </c>
@@ -6022,7 +6040,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>52</v>
       </c>
@@ -6045,7 +6063,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>52</v>
       </c>
@@ -6068,7 +6086,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>52</v>
       </c>
@@ -6091,7 +6109,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>52</v>
       </c>
@@ -6114,7 +6132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>52</v>
       </c>
@@ -6137,7 +6155,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>54</v>
       </c>
@@ -6160,7 +6178,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>54</v>
       </c>
@@ -6183,7 +6201,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>54</v>
       </c>
@@ -6206,7 +6224,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>54</v>
       </c>
@@ -6229,7 +6247,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>54</v>
       </c>
@@ -6252,7 +6270,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>54</v>
       </c>
@@ -6275,7 +6293,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>54</v>
       </c>
@@ -6298,7 +6316,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>54</v>
       </c>
@@ -6321,7 +6339,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>54</v>
       </c>
@@ -6344,7 +6362,7 @@
         <v>57.9</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>54</v>
       </c>
@@ -6367,7 +6385,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>54</v>
       </c>
@@ -6390,7 +6408,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>54</v>
       </c>
@@ -6413,7 +6431,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>54</v>
       </c>
@@ -6436,7 +6454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>54</v>
       </c>
@@ -6459,7 +6477,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>54</v>
       </c>
@@ -6482,7 +6500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>56</v>
       </c>
@@ -6505,7 +6523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>56</v>
       </c>
@@ -6528,7 +6546,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>56</v>
       </c>
@@ -6551,7 +6569,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>56</v>
       </c>
@@ -6574,7 +6592,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>56</v>
       </c>
@@ -6597,7 +6615,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>56</v>
       </c>
@@ -6620,7 +6638,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>56</v>
       </c>
@@ -6643,7 +6661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>56</v>
       </c>
@@ -6666,7 +6684,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>56</v>
       </c>
@@ -6689,7 +6707,7 @@
         <v>60.6</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>56</v>
       </c>
@@ -6712,7 +6730,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>56</v>
       </c>
@@ -6735,7 +6753,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>56</v>
       </c>
@@ -6758,7 +6776,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>56</v>
       </c>
@@ -6781,7 +6799,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>56</v>
       </c>
@@ -6804,7 +6822,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>56</v>
       </c>
@@ -6827,7 +6845,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>58</v>
       </c>
@@ -6850,7 +6868,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>58</v>
       </c>
@@ -6873,7 +6891,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>58</v>
       </c>
@@ -6896,7 +6914,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>58</v>
       </c>
@@ -6919,7 +6937,7 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>58</v>
       </c>
@@ -6942,7 +6960,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>58</v>
       </c>
@@ -6965,7 +6983,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>58</v>
       </c>
@@ -6988,7 +7006,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>58</v>
       </c>
@@ -7011,7 +7029,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>58</v>
       </c>
@@ -7034,7 +7052,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>58</v>
       </c>
@@ -7057,7 +7075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>58</v>
       </c>
@@ -7080,7 +7098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>58</v>
       </c>
@@ -7103,7 +7121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>58</v>
       </c>
@@ -7126,7 +7144,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>58</v>
       </c>
@@ -7149,7 +7167,7 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>58</v>
       </c>
@@ -7172,7 +7190,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>60</v>
       </c>
@@ -7195,7 +7213,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>60</v>
       </c>
@@ -7218,7 +7236,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>60</v>
       </c>
@@ -7241,7 +7259,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>60</v>
       </c>
@@ -7264,7 +7282,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>60</v>
       </c>
@@ -7287,7 +7305,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>60</v>
       </c>
@@ -7310,7 +7328,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>60</v>
       </c>
@@ -7333,7 +7351,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>60</v>
       </c>
@@ -7356,7 +7374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>60</v>
       </c>
@@ -7379,7 +7397,7 @@
         <v>69.7</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>60</v>
       </c>
@@ -7402,7 +7420,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>60</v>
       </c>
@@ -7425,7 +7443,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>60</v>
       </c>
@@ -7448,7 +7466,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>60</v>
       </c>
@@ -7471,7 +7489,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>60</v>
       </c>
@@ -7494,7 +7512,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>60</v>
       </c>
@@ -7517,7 +7535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>62</v>
       </c>
@@ -7540,7 +7558,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>62</v>
       </c>
@@ -7563,7 +7581,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>62</v>
       </c>
@@ -7586,7 +7604,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>62</v>
       </c>
@@ -7609,7 +7627,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>62</v>
       </c>
@@ -7632,7 +7650,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>62</v>
       </c>
@@ -7655,7 +7673,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>62</v>
       </c>
@@ -7678,7 +7696,7 @@
         <v>47.8</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>62</v>
       </c>
@@ -7701,7 +7719,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>62</v>
       </c>
@@ -7724,7 +7742,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>62</v>
       </c>
@@ -7747,7 +7765,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>62</v>
       </c>
@@ -7770,7 +7788,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>62</v>
       </c>
@@ -7793,7 +7811,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>65</v>
       </c>
@@ -7816,7 +7834,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>65</v>
       </c>
@@ -7839,7 +7857,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>65</v>
       </c>
@@ -7862,7 +7880,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>65</v>
       </c>
@@ -7885,7 +7903,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>65</v>
       </c>
@@ -7908,7 +7926,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>65</v>
       </c>
@@ -7931,7 +7949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>65</v>
       </c>
@@ -7954,7 +7972,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>65</v>
       </c>
@@ -7977,7 +7995,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>65</v>
       </c>
@@ -8000,7 +8018,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>65</v>
       </c>
@@ -8023,7 +8041,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>65</v>
       </c>
@@ -8046,7 +8064,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>65</v>
       </c>
@@ -8069,7 +8087,7 @@
         <v>59.6</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>68</v>
       </c>
@@ -8092,7 +8110,7 @@
         <v>40.700000000000003</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>68</v>
       </c>
@@ -8115,7 +8133,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>68</v>
       </c>
@@ -8138,7 +8156,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>68</v>
       </c>
@@ -8161,7 +8179,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>68</v>
       </c>
@@ -8184,7 +8202,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>68</v>
       </c>
@@ -8207,7 +8225,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>68</v>
       </c>
@@ -8230,7 +8248,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>68</v>
       </c>
@@ -8253,7 +8271,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>68</v>
       </c>
@@ -8276,7 +8294,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>68</v>
       </c>
@@ -8299,7 +8317,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>68</v>
       </c>
@@ -8322,7 +8340,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>68</v>
       </c>
@@ -8345,7 +8363,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>71</v>
       </c>
@@ -8368,7 +8386,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>71</v>
       </c>
@@ -8391,7 +8409,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>71</v>
       </c>
@@ -8414,7 +8432,7 @@
         <v>51.7</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>71</v>
       </c>
@@ -8437,7 +8455,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>71</v>
       </c>
@@ -8460,7 +8478,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>71</v>
       </c>
@@ -8483,7 +8501,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>71</v>
       </c>
@@ -8506,7 +8524,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>71</v>
       </c>
@@ -8529,7 +8547,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>71</v>
       </c>
@@ -8552,7 +8570,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>71</v>
       </c>
@@ -8575,7 +8593,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>71</v>
       </c>
@@ -8598,7 +8616,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>71</v>
       </c>
@@ -8621,7 +8639,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>74</v>
       </c>
@@ -8644,7 +8662,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>74</v>
       </c>
@@ -8667,7 +8685,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>74</v>
       </c>
@@ -8690,7 +8708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>74</v>
       </c>
@@ -8713,7 +8731,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>74</v>
       </c>
@@ -8736,7 +8754,7 @@
         <v>69.7</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>74</v>
       </c>
@@ -8759,7 +8777,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>74</v>
       </c>
@@ -8782,7 +8800,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>74</v>
       </c>
@@ -8805,7 +8823,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>74</v>
       </c>
@@ -8828,7 +8846,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>74</v>
       </c>
@@ -8851,7 +8869,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>74</v>
       </c>
@@ -8874,7 +8892,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>74</v>
       </c>
@@ -8897,7 +8915,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>74</v>
       </c>
@@ -8920,7 +8938,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>74</v>
       </c>
@@ -8943,7 +8961,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>74</v>
       </c>
@@ -8966,7 +8984,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>81</v>
       </c>
@@ -8989,7 +9007,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>81</v>
       </c>
@@ -9012,7 +9030,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>81</v>
       </c>
@@ -9035,7 +9053,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>81</v>
       </c>
@@ -9058,7 +9076,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>81</v>
       </c>
@@ -9081,7 +9099,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>81</v>
       </c>
@@ -9104,7 +9122,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>81</v>
       </c>
@@ -9127,7 +9145,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>81</v>
       </c>
@@ -9150,7 +9168,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>81</v>
       </c>
@@ -9173,7 +9191,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>81</v>
       </c>
@@ -9196,7 +9214,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>81</v>
       </c>
@@ -9219,7 +9237,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>81</v>
       </c>
@@ -9242,7 +9260,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>81</v>
       </c>
@@ -9265,7 +9283,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>81</v>
       </c>
@@ -9288,7 +9306,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>81</v>
       </c>
@@ -9515,7 +9533,7 @@
         <v>85</v>
       </c>
       <c r="G385">
-        <v>38.799999999999997</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
@@ -9588,6 +9606,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G388" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DailyAct_22"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>